<commit_message>
Tests angepasst. Alle laufen durch
</commit_message>
<xml_diff>
--- a/src/main/2 insert Sozialversicherungsdaten/2 gesetzliche Krankenkasse.xlsx
+++ b/src/main/2 insert Sozialversicherungsdaten/2 gesetzliche Krankenkasse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\2 insert Sozialversicherungsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B1CF13-BF3E-4A5E-A194-4E179A160D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7BDD38-BAF6-481F-9335-1B53A757255A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2292" yWindow="1752" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34830" yWindow="4800" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Daten</t>
   </si>
@@ -42,18 +42,12 @@
     <t>KKH</t>
   </si>
   <si>
-    <t>Zusatzbeitrag Krankenversicherung in Prozent</t>
-  </si>
-  <si>
     <t>Kaufmaennische Krankenkasse</t>
   </si>
   <si>
     <t>Eintragungsdatum</t>
   </si>
   <si>
-    <t>15.12.2023</t>
-  </si>
-  <si>
     <t>Umlage U1 in Prozent</t>
   </si>
   <si>
@@ -61,6 +55,15 @@
   </si>
   <si>
     <t>Insolvenzgeldumlage</t>
+  </si>
+  <si>
+    <t>Zusatzbeitrag Krankenversicherung AG-Anteil in Prozent</t>
+  </si>
+  <si>
+    <t>Zusatzbeitrag Krankenversicherung AN-Anteil in Prozent</t>
+  </si>
+  <si>
+    <t>01.01.2024</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -427,42 +430,50 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
-        <v>1.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
-        <v>2.2999999999999998</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>0.44</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>0.06</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>